<commit_message>
commiting searching and sorting for all models
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533487\Documents\44663\Team07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531378\Documents\44663\Team07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -1484,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,7 +1994,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>